<commit_message>
Update to docs new scripts and started manuscript text.
</commit_message>
<xml_diff>
--- a/metadata/raw_sample_metadata.xlsx
+++ b/metadata/raw_sample_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f19994348ecc0c8c/Documents/GitHub/uwa_darwins_daisy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{61D53B89-ACC9-B949-A960-2A8792D0D97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{045BB79E-7D80-4928-AA88-A8A965C8895E}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="13_ncr:1_{61D53B89-ACC9-B949-A960-2A8792D0D97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4EFDFB3-82DA-4088-BC07-4089E87FF0BA}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="S1 Sample Overview" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'S1 Sample Overview'!$A$1:$M$410</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'S1 Sample Overview'!$A$1:$M$409</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="152">
   <si>
     <t>sampleID</t>
   </si>
@@ -509,19 +509,7 @@
     <t>ERR12356073, ERR12356079</t>
   </si>
   <si>
-    <t>HAMP24</t>
-  </si>
-  <si>
     <t>Scalesia villosa</t>
-  </si>
-  <si>
-    <t>Champion</t>
-  </si>
-  <si>
-    <t>HAMP24_2</t>
-  </si>
-  <si>
-    <t>ERR12360771</t>
   </si>
   <si>
     <t>HAMP28</t>
@@ -611,7 +599,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -639,12 +627,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -769,8 +751,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -778,8 +760,7 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,13 +979,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q746"/>
+  <dimension ref="A1:Q745"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1079,7 +1060,7 @@
       <c r="D2" s="8">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="15">
@@ -1118,7 +1099,7 @@
       <c r="D3" s="8">
         <v>6</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F3" s="15">
@@ -1157,7 +1138,7 @@
       <c r="D4" s="8">
         <v>6</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F4" s="15">
@@ -1196,7 +1177,7 @@
       <c r="D5" s="8">
         <v>6</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F5" s="15">
@@ -1235,7 +1216,7 @@
       <c r="D6" s="8">
         <v>6</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F6" s="15">
@@ -1274,7 +1255,7 @@
       <c r="D7" s="8">
         <v>6</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="F7" s="15">
@@ -1391,7 +1372,7 @@
       <c r="D10" s="8">
         <v>3</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="15">
@@ -1434,7 +1415,7 @@
       <c r="D11" s="8">
         <v>3</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>141</v>
       </c>
       <c r="F11" s="15">
@@ -1477,7 +1458,7 @@
       <c r="D12" s="8">
         <v>3</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="15">
@@ -1520,7 +1501,7 @@
       <c r="D13" s="8">
         <v>4</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="26" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="15">
@@ -1640,7 +1621,7 @@
       <c r="A16" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -1649,7 +1630,7 @@
       <c r="D16" s="8">
         <v>2</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="15">
@@ -1681,7 +1662,7 @@
       <c r="A17" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1690,7 +1671,7 @@
       <c r="D17" s="8">
         <v>2</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="15">
@@ -1724,7 +1705,7 @@
       <c r="A18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1733,7 +1714,7 @@
       <c r="D18" s="8">
         <v>2</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="15">
@@ -1862,7 +1843,7 @@
       <c r="D21" s="8">
         <v>4</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>104</v>
       </c>
       <c r="F21" s="15">
@@ -1979,42 +1960,42 @@
       <c r="Q23" s="14"/>
     </row>
     <row r="24" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
-        <v>150</v>
+      <c r="A24" s="19" t="s">
+        <v>149</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="D24" s="8">
-        <v>0</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>149</v>
+        <v>5</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="F24" s="15">
         <v>35815</v>
       </c>
       <c r="G24" s="12">
-        <v>-1.2372209999999999</v>
+        <v>-1.2252780000000001</v>
       </c>
       <c r="H24" s="12">
-        <v>-90.385727000000003</v>
+        <v>-90.427778000000004</v>
       </c>
       <c r="I24" s="12">
-        <v>8.7117799999999992</v>
+        <v>13.6873</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L24" s="8"/>
       <c r="M24" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
@@ -2022,42 +2003,42 @@
       <c r="Q24" s="14"/>
     </row>
     <row r="25" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
-        <v>153</v>
+      <c r="A25" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>148</v>
+        <v>16</v>
       </c>
       <c r="D25" s="8">
         <v>5</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="15">
-        <v>35815</v>
+        <v>35816</v>
       </c>
       <c r="G25" s="12">
-        <v>-1.2252780000000001</v>
+        <v>-1.282778</v>
       </c>
       <c r="H25" s="12">
-        <v>-90.427778000000004</v>
+        <v>-90.491388999999998</v>
       </c>
       <c r="I25" s="12">
-        <v>13.6873</v>
+        <v>12.360900000000001</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="9" t="s">
-        <v>154</v>
+        <v>25</v>
       </c>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
@@ -2066,41 +2047,41 @@
     </row>
     <row r="26" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D26" s="8">
         <v>5</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F26" s="15">
         <v>35816</v>
       </c>
       <c r="G26" s="12">
-        <v>-1.282778</v>
+        <v>-1.291944</v>
       </c>
       <c r="H26" s="12">
-        <v>-90.491388999999998</v>
+        <v>-90.453056000000004</v>
       </c>
       <c r="I26" s="12">
-        <v>12.360900000000001</v>
+        <v>14.399699999999999</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="9" t="s">
-        <v>25</v>
+        <v>123</v>
       </c>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
@@ -2109,41 +2090,39 @@
     </row>
     <row r="27" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>120</v>
       </c>
       <c r="D27" s="8">
-        <v>5</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="F27" s="15">
-        <v>35816</v>
+        <v>35820</v>
       </c>
       <c r="G27" s="12">
-        <v>-1.291944</v>
+        <v>-0.901111</v>
       </c>
       <c r="H27" s="12">
-        <v>-90.453056000000004</v>
+        <v>-89.439722000000003</v>
       </c>
       <c r="I27" s="12">
-        <v>14.399699999999999</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>57</v>
-      </c>
+        <v>13.2997</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" s="6"/>
       <c r="L27" s="8"/>
       <c r="M27" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
@@ -2152,39 +2131,41 @@
     </row>
     <row r="28" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D28" s="8">
         <v>6</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F28" s="15">
-        <v>35820</v>
+        <v>35821</v>
       </c>
       <c r="G28" s="12">
-        <v>-0.901111</v>
+        <v>-0.93027800000000005</v>
       </c>
       <c r="H28" s="12">
-        <v>-89.439722000000003</v>
+        <v>-89.608056000000005</v>
       </c>
       <c r="I28" s="12">
-        <v>13.2997</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="6"/>
+        <v>14.261100000000001</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="L28" s="8"/>
       <c r="M28" s="9" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
@@ -2193,31 +2174,31 @@
     </row>
     <row r="29" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="D29" s="8">
-        <v>6</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>81</v>
+        <v>4</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="F29" s="15">
-        <v>35821</v>
+        <v>35809</v>
       </c>
       <c r="G29" s="12">
-        <v>-0.93027800000000005</v>
+        <v>-0.73777800000000004</v>
       </c>
       <c r="H29" s="12">
-        <v>-89.608056000000005</v>
+        <v>-90.324444</v>
       </c>
       <c r="I29" s="12">
-        <v>14.261100000000001</v>
+        <v>13.123100000000001</v>
       </c>
       <c r="J29" s="13" t="s">
         <v>15</v>
@@ -2227,7 +2208,7 @@
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="9" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
@@ -2236,41 +2217,41 @@
     </row>
     <row r="30" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="D30" s="8">
-        <v>4</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="F30" s="15">
-        <v>35809</v>
+        <v>35822</v>
       </c>
       <c r="G30" s="12">
-        <v>-0.73777800000000004</v>
+        <v>-0.71166700000000005</v>
       </c>
       <c r="H30" s="12">
-        <v>-90.324444</v>
+        <v>-89.247500000000002</v>
       </c>
       <c r="I30" s="12">
-        <v>13.123100000000001</v>
+        <v>12.0222</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L30" s="8"/>
       <c r="M30" s="9" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="N30" s="14"/>
       <c r="O30" s="14"/>
@@ -2279,41 +2260,41 @@
     </row>
     <row r="31" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="D31" s="8">
-        <v>6</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>81</v>
+        <v>4</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="F31" s="15">
-        <v>35822</v>
+        <v>35810</v>
       </c>
       <c r="G31" s="12">
-        <v>-0.71166700000000005</v>
+        <v>-0.48991699999999999</v>
       </c>
       <c r="H31" s="12">
-        <v>-89.247500000000002</v>
+        <v>-90.280249999999995</v>
       </c>
       <c r="I31" s="12">
-        <v>12.0222</v>
+        <v>13.773899999999999</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K31" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L31" s="8"/>
       <c r="M31" s="9" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="N31" s="14"/>
       <c r="O31" s="14"/>
@@ -2322,13 +2303,13 @@
     </row>
     <row r="32" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D32" s="8">
         <v>4</v>
@@ -2340,13 +2321,13 @@
         <v>35810</v>
       </c>
       <c r="G32" s="12">
-        <v>-0.48991699999999999</v>
+        <v>-0.54666700000000001</v>
       </c>
       <c r="H32" s="12">
-        <v>-90.280249999999995</v>
+        <v>-90.319166999999993</v>
       </c>
       <c r="I32" s="12">
-        <v>13.773899999999999</v>
+        <v>15.8598</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>15</v>
@@ -2356,7 +2337,7 @@
       </c>
       <c r="L32" s="8"/>
       <c r="M32" s="9" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
@@ -2365,13 +2346,13 @@
     </row>
     <row r="33" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="D33" s="8">
         <v>4</v>
@@ -2380,16 +2361,16 @@
         <v>19</v>
       </c>
       <c r="F33" s="15">
-        <v>35810</v>
+        <v>36921</v>
       </c>
       <c r="G33" s="12">
-        <v>-0.54666700000000001</v>
+        <v>-0.71294999999999997</v>
       </c>
       <c r="H33" s="12">
-        <v>-90.319166999999993</v>
+        <v>-90.226892000000007</v>
       </c>
       <c r="I33" s="12">
-        <v>15.8598</v>
+        <v>13.0764</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>15</v>
@@ -2399,7 +2380,7 @@
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="9" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>
@@ -2408,41 +2389,41 @@
     </row>
     <row r="34" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>137</v>
+        <v>53</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="D34" s="8">
-        <v>4</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="F34" s="15">
-        <v>36921</v>
+        <v>36536</v>
       </c>
       <c r="G34" s="12">
-        <v>-0.71294999999999997</v>
+        <v>0.54157200000000005</v>
       </c>
       <c r="H34" s="12">
-        <v>-90.226892000000007</v>
+        <v>-90.741054000000005</v>
       </c>
       <c r="I34" s="12">
-        <v>13.0764</v>
+        <v>15.1455</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L34" s="8"/>
       <c r="M34" s="9" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
@@ -2451,10 +2432,10 @@
     </row>
     <row r="35" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>51</v>
@@ -2466,26 +2447,26 @@
         <v>52</v>
       </c>
       <c r="F35" s="15">
-        <v>36536</v>
+        <v>36541</v>
       </c>
       <c r="G35" s="12">
-        <v>0.54157200000000005</v>
+        <v>0.57333299999999998</v>
       </c>
       <c r="H35" s="12">
-        <v>-90.741054000000005</v>
+        <v>-90.764388999999994</v>
       </c>
       <c r="I35" s="12">
-        <v>15.1455</v>
+        <v>15.824199999999999</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="L35" s="8"/>
       <c r="M35" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
@@ -2493,43 +2474,19 @@
       <c r="Q35" s="14"/>
     </row>
     <row r="36" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="8">
-        <v>1</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="15">
-        <v>36541</v>
-      </c>
-      <c r="G36" s="12">
-        <v>0.57333299999999998</v>
-      </c>
-      <c r="H36" s="12">
-        <v>-90.764388999999994</v>
-      </c>
-      <c r="I36" s="12">
-        <v>15.824199999999999</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="M36" s="9"/>
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
@@ -3034,7 +2991,7 @@
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="E63" s="16"/>
       <c r="F63" s="15"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
@@ -3053,7 +3010,7 @@
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
-      <c r="E64" s="16"/>
+      <c r="E64" s="8"/>
       <c r="F64" s="15"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -3229,8 +3186,8 @@
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
       <c r="L73" s="8"/>
       <c r="M73" s="9"/>
       <c r="N73" s="14"/>
@@ -3248,8 +3205,8 @@
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
       <c r="L74" s="8"/>
       <c r="M74" s="9"/>
       <c r="N74" s="14"/>
@@ -3932,8 +3889,8 @@
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
-      <c r="J110" s="13"/>
-      <c r="K110" s="13"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
       <c r="L110" s="8"/>
       <c r="M110" s="9"/>
       <c r="N110" s="14"/>
@@ -3951,8 +3908,8 @@
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
-      <c r="J111" s="6"/>
-      <c r="K111" s="6"/>
+      <c r="J111" s="13"/>
+      <c r="K111" s="13"/>
       <c r="L111" s="8"/>
       <c r="M111" s="9"/>
       <c r="N111" s="14"/>
@@ -4255,8 +4212,8 @@
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
       <c r="I127" s="12"/>
-      <c r="J127" s="13"/>
-      <c r="K127" s="13"/>
+      <c r="J127" s="6"/>
+      <c r="K127" s="6"/>
       <c r="L127" s="8"/>
       <c r="M127" s="9"/>
       <c r="N127" s="14"/>
@@ -4274,8 +4231,8 @@
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
       <c r="I128" s="12"/>
-      <c r="J128" s="6"/>
-      <c r="K128" s="6"/>
+      <c r="J128" s="13"/>
+      <c r="K128" s="13"/>
       <c r="L128" s="8"/>
       <c r="M128" s="9"/>
       <c r="N128" s="14"/>
@@ -4312,8 +4269,8 @@
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
       <c r="I130" s="12"/>
-      <c r="J130" s="13"/>
-      <c r="K130" s="13"/>
+      <c r="J130" s="6"/>
+      <c r="K130" s="6"/>
       <c r="L130" s="8"/>
       <c r="M130" s="9"/>
       <c r="N130" s="14"/>
@@ -4331,8 +4288,8 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
-      <c r="J131" s="6"/>
-      <c r="K131" s="6"/>
+      <c r="J131" s="13"/>
+      <c r="K131" s="13"/>
       <c r="L131" s="8"/>
       <c r="M131" s="9"/>
       <c r="N131" s="14"/>
@@ -4364,7 +4321,7 @@
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
+      <c r="E133" s="16"/>
       <c r="F133" s="15"/>
       <c r="G133" s="12"/>
       <c r="H133" s="12"/>
@@ -4383,7 +4340,7 @@
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
-      <c r="E134" s="16"/>
+      <c r="E134" s="8"/>
       <c r="F134" s="15"/>
       <c r="G134" s="12"/>
       <c r="H134" s="12"/>
@@ -5010,7 +4967,7 @@
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
       <c r="D167" s="8"/>
-      <c r="E167" s="8"/>
+      <c r="E167" s="16"/>
       <c r="F167" s="15"/>
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
@@ -5029,7 +4986,7 @@
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
       <c r="D168" s="8"/>
-      <c r="E168" s="16"/>
+      <c r="E168" s="8"/>
       <c r="F168" s="15"/>
       <c r="G168" s="12"/>
       <c r="H168" s="12"/>
@@ -5167,8 +5124,8 @@
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
       <c r="I175" s="12"/>
-      <c r="J175" s="13"/>
-      <c r="K175" s="13"/>
+      <c r="J175" s="6"/>
+      <c r="K175" s="6"/>
       <c r="L175" s="8"/>
       <c r="M175" s="9"/>
       <c r="N175" s="14"/>
@@ -5186,8 +5143,8 @@
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
       <c r="I176" s="12"/>
-      <c r="J176" s="6"/>
-      <c r="K176" s="6"/>
+      <c r="J176" s="13"/>
+      <c r="K176" s="13"/>
       <c r="L176" s="8"/>
       <c r="M176" s="9"/>
       <c r="N176" s="14"/>
@@ -5200,7 +5157,7 @@
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
       <c r="D177" s="8"/>
-      <c r="E177" s="8"/>
+      <c r="E177" s="16"/>
       <c r="F177" s="15"/>
       <c r="G177" s="12"/>
       <c r="H177" s="12"/>
@@ -5219,7 +5176,7 @@
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
       <c r="D178" s="8"/>
-      <c r="E178" s="16"/>
+      <c r="E178" s="8"/>
       <c r="F178" s="15"/>
       <c r="G178" s="12"/>
       <c r="H178" s="12"/>
@@ -5789,7 +5746,7 @@
       <c r="B208" s="8"/>
       <c r="C208" s="8"/>
       <c r="D208" s="8"/>
-      <c r="E208" s="8"/>
+      <c r="E208" s="16"/>
       <c r="F208" s="15"/>
       <c r="G208" s="12"/>
       <c r="H208" s="12"/>
@@ -5808,7 +5765,7 @@
       <c r="B209" s="8"/>
       <c r="C209" s="8"/>
       <c r="D209" s="8"/>
-      <c r="E209" s="16"/>
+      <c r="E209" s="8"/>
       <c r="F209" s="15"/>
       <c r="G209" s="12"/>
       <c r="H209" s="12"/>
@@ -5922,7 +5879,7 @@
       <c r="B215" s="8"/>
       <c r="C215" s="8"/>
       <c r="D215" s="8"/>
-      <c r="E215" s="8"/>
+      <c r="E215" s="16"/>
       <c r="F215" s="15"/>
       <c r="G215" s="12"/>
       <c r="H215" s="12"/>
@@ -5941,7 +5898,7 @@
       <c r="B216" s="8"/>
       <c r="C216" s="8"/>
       <c r="D216" s="8"/>
-      <c r="E216" s="16"/>
+      <c r="E216" s="8"/>
       <c r="F216" s="15"/>
       <c r="G216" s="12"/>
       <c r="H216" s="12"/>
@@ -6150,7 +6107,7 @@
       <c r="B227" s="8"/>
       <c r="C227" s="8"/>
       <c r="D227" s="8"/>
-      <c r="E227" s="8"/>
+      <c r="E227" s="16"/>
       <c r="F227" s="15"/>
       <c r="G227" s="12"/>
       <c r="H227" s="12"/>
@@ -6169,7 +6126,7 @@
       <c r="B228" s="8"/>
       <c r="C228" s="8"/>
       <c r="D228" s="8"/>
-      <c r="E228" s="16"/>
+      <c r="E228" s="8"/>
       <c r="F228" s="15"/>
       <c r="G228" s="12"/>
       <c r="H228" s="12"/>
@@ -6511,7 +6468,7 @@
       <c r="B246" s="8"/>
       <c r="C246" s="8"/>
       <c r="D246" s="8"/>
-      <c r="E246" s="8"/>
+      <c r="E246" s="16"/>
       <c r="F246" s="15"/>
       <c r="G246" s="12"/>
       <c r="H246" s="12"/>
@@ -6530,7 +6487,7 @@
       <c r="B247" s="8"/>
       <c r="C247" s="8"/>
       <c r="D247" s="8"/>
-      <c r="E247" s="16"/>
+      <c r="E247" s="8"/>
       <c r="F247" s="15"/>
       <c r="G247" s="12"/>
       <c r="H247" s="12"/>
@@ -6815,7 +6772,7 @@
       <c r="B262" s="8"/>
       <c r="C262" s="8"/>
       <c r="D262" s="8"/>
-      <c r="E262" s="8"/>
+      <c r="E262" s="16"/>
       <c r="F262" s="15"/>
       <c r="G262" s="12"/>
       <c r="H262" s="12"/>
@@ -6834,7 +6791,7 @@
       <c r="B263" s="8"/>
       <c r="C263" s="8"/>
       <c r="D263" s="8"/>
-      <c r="E263" s="16"/>
+      <c r="E263" s="8"/>
       <c r="F263" s="15"/>
       <c r="G263" s="12"/>
       <c r="H263" s="12"/>
@@ -7162,8 +7119,8 @@
       <c r="G280" s="12"/>
       <c r="H280" s="12"/>
       <c r="I280" s="12"/>
-      <c r="J280" s="13"/>
-      <c r="K280" s="13"/>
+      <c r="J280" s="6"/>
+      <c r="K280" s="6"/>
       <c r="L280" s="8"/>
       <c r="M280" s="9"/>
       <c r="N280" s="14"/>
@@ -7181,8 +7138,8 @@
       <c r="G281" s="12"/>
       <c r="H281" s="12"/>
       <c r="I281" s="12"/>
-      <c r="J281" s="6"/>
-      <c r="K281" s="6"/>
+      <c r="J281" s="13"/>
+      <c r="K281" s="13"/>
       <c r="L281" s="8"/>
       <c r="M281" s="9"/>
       <c r="N281" s="14"/>
@@ -7447,8 +7404,8 @@
       <c r="G295" s="12"/>
       <c r="H295" s="12"/>
       <c r="I295" s="12"/>
-      <c r="J295" s="13"/>
-      <c r="K295" s="13"/>
+      <c r="J295" s="6"/>
+      <c r="K295" s="6"/>
       <c r="L295" s="8"/>
       <c r="M295" s="9"/>
       <c r="N295" s="14"/>
@@ -7485,8 +7442,8 @@
       <c r="G297" s="12"/>
       <c r="H297" s="12"/>
       <c r="I297" s="12"/>
-      <c r="J297" s="6"/>
-      <c r="K297" s="6"/>
+      <c r="J297" s="13"/>
+      <c r="K297" s="13"/>
       <c r="L297" s="8"/>
       <c r="M297" s="9"/>
       <c r="N297" s="14"/>
@@ -7599,8 +7556,8 @@
       <c r="G303" s="12"/>
       <c r="H303" s="12"/>
       <c r="I303" s="12"/>
-      <c r="J303" s="13"/>
-      <c r="K303" s="13"/>
+      <c r="J303" s="6"/>
+      <c r="K303" s="6"/>
       <c r="L303" s="8"/>
       <c r="M303" s="9"/>
       <c r="N303" s="14"/>
@@ -7618,8 +7575,8 @@
       <c r="G304" s="12"/>
       <c r="H304" s="12"/>
       <c r="I304" s="12"/>
-      <c r="J304" s="6"/>
-      <c r="K304" s="6"/>
+      <c r="J304" s="13"/>
+      <c r="K304" s="13"/>
       <c r="L304" s="8"/>
       <c r="M304" s="9"/>
       <c r="N304" s="14"/>
@@ -7656,8 +7613,8 @@
       <c r="G306" s="12"/>
       <c r="H306" s="12"/>
       <c r="I306" s="12"/>
-      <c r="J306" s="13"/>
-      <c r="K306" s="13"/>
+      <c r="J306" s="6"/>
+      <c r="K306" s="6"/>
       <c r="L306" s="8"/>
       <c r="M306" s="9"/>
       <c r="N306" s="14"/>
@@ -7675,8 +7632,8 @@
       <c r="G307" s="12"/>
       <c r="H307" s="12"/>
       <c r="I307" s="12"/>
-      <c r="J307" s="6"/>
-      <c r="K307" s="6"/>
+      <c r="J307" s="13"/>
+      <c r="K307" s="13"/>
       <c r="L307" s="8"/>
       <c r="M307" s="9"/>
       <c r="N307" s="14"/>
@@ -7732,8 +7689,8 @@
       <c r="G310" s="12"/>
       <c r="H310" s="12"/>
       <c r="I310" s="12"/>
-      <c r="J310" s="13"/>
-      <c r="K310" s="13"/>
+      <c r="J310" s="6"/>
+      <c r="K310" s="6"/>
       <c r="L310" s="8"/>
       <c r="M310" s="9"/>
       <c r="N310" s="14"/>
@@ -7751,8 +7708,8 @@
       <c r="G311" s="12"/>
       <c r="H311" s="12"/>
       <c r="I311" s="12"/>
-      <c r="J311" s="6"/>
-      <c r="K311" s="6"/>
+      <c r="J311" s="13"/>
+      <c r="K311" s="13"/>
       <c r="L311" s="8"/>
       <c r="M311" s="9"/>
       <c r="N311" s="14"/>
@@ -7960,8 +7917,8 @@
       <c r="G322" s="12"/>
       <c r="H322" s="12"/>
       <c r="I322" s="12"/>
-      <c r="J322" s="13"/>
-      <c r="K322" s="13"/>
+      <c r="J322" s="6"/>
+      <c r="K322" s="6"/>
       <c r="L322" s="8"/>
       <c r="M322" s="9"/>
       <c r="N322" s="14"/>
@@ -7979,8 +7936,8 @@
       <c r="G323" s="12"/>
       <c r="H323" s="12"/>
       <c r="I323" s="12"/>
-      <c r="J323" s="6"/>
-      <c r="K323" s="6"/>
+      <c r="J323" s="13"/>
+      <c r="K323" s="13"/>
       <c r="L323" s="8"/>
       <c r="M323" s="9"/>
       <c r="N323" s="14"/>
@@ -8055,8 +8012,8 @@
       <c r="G327" s="12"/>
       <c r="H327" s="12"/>
       <c r="I327" s="12"/>
-      <c r="J327" s="13"/>
-      <c r="K327" s="13"/>
+      <c r="J327" s="6"/>
+      <c r="K327" s="6"/>
       <c r="L327" s="8"/>
       <c r="M327" s="9"/>
       <c r="N327" s="14"/>
@@ -8074,8 +8031,8 @@
       <c r="G328" s="12"/>
       <c r="H328" s="12"/>
       <c r="I328" s="12"/>
-      <c r="J328" s="6"/>
-      <c r="K328" s="6"/>
+      <c r="J328" s="13"/>
+      <c r="K328" s="13"/>
       <c r="L328" s="8"/>
       <c r="M328" s="9"/>
       <c r="N328" s="14"/>
@@ -8131,8 +8088,8 @@
       <c r="G331" s="12"/>
       <c r="H331" s="12"/>
       <c r="I331" s="12"/>
-      <c r="J331" s="13"/>
-      <c r="K331" s="13"/>
+      <c r="J331" s="6"/>
+      <c r="K331" s="6"/>
       <c r="L331" s="8"/>
       <c r="M331" s="9"/>
       <c r="N331" s="14"/>
@@ -8150,8 +8107,8 @@
       <c r="G332" s="12"/>
       <c r="H332" s="12"/>
       <c r="I332" s="12"/>
-      <c r="J332" s="6"/>
-      <c r="K332" s="6"/>
+      <c r="J332" s="13"/>
+      <c r="K332" s="13"/>
       <c r="L332" s="8"/>
       <c r="M332" s="9"/>
       <c r="N332" s="14"/>
@@ -8226,8 +8183,8 @@
       <c r="G336" s="12"/>
       <c r="H336" s="12"/>
       <c r="I336" s="12"/>
-      <c r="J336" s="13"/>
-      <c r="K336" s="13"/>
+      <c r="J336" s="6"/>
+      <c r="K336" s="6"/>
       <c r="L336" s="8"/>
       <c r="M336" s="9"/>
       <c r="N336" s="14"/>
@@ -8245,8 +8202,8 @@
       <c r="G337" s="12"/>
       <c r="H337" s="12"/>
       <c r="I337" s="12"/>
-      <c r="J337" s="6"/>
-      <c r="K337" s="6"/>
+      <c r="J337" s="13"/>
+      <c r="K337" s="13"/>
       <c r="L337" s="8"/>
       <c r="M337" s="9"/>
       <c r="N337" s="14"/>
@@ -8264,8 +8221,8 @@
       <c r="G338" s="12"/>
       <c r="H338" s="12"/>
       <c r="I338" s="12"/>
-      <c r="J338" s="13"/>
-      <c r="K338" s="13"/>
+      <c r="J338" s="6"/>
+      <c r="K338" s="6"/>
       <c r="L338" s="8"/>
       <c r="M338" s="9"/>
       <c r="N338" s="14"/>
@@ -8283,8 +8240,8 @@
       <c r="G339" s="12"/>
       <c r="H339" s="12"/>
       <c r="I339" s="12"/>
-      <c r="J339" s="6"/>
-      <c r="K339" s="6"/>
+      <c r="J339" s="13"/>
+      <c r="K339" s="13"/>
       <c r="L339" s="8"/>
       <c r="M339" s="9"/>
       <c r="N339" s="14"/>
@@ -8336,7 +8293,7 @@
       <c r="C342" s="8"/>
       <c r="D342" s="8"/>
       <c r="E342" s="8"/>
-      <c r="F342" s="15"/>
+      <c r="F342" s="11"/>
       <c r="G342" s="12"/>
       <c r="H342" s="12"/>
       <c r="I342" s="12"/>
@@ -8355,7 +8312,7 @@
       <c r="C343" s="8"/>
       <c r="D343" s="8"/>
       <c r="E343" s="8"/>
-      <c r="F343" s="11"/>
+      <c r="F343" s="15"/>
       <c r="G343" s="12"/>
       <c r="H343" s="12"/>
       <c r="I343" s="12"/>
@@ -8393,7 +8350,7 @@
       <c r="C345" s="8"/>
       <c r="D345" s="8"/>
       <c r="E345" s="8"/>
-      <c r="F345" s="15"/>
+      <c r="F345" s="11"/>
       <c r="G345" s="12"/>
       <c r="H345" s="12"/>
       <c r="I345" s="12"/>
@@ -8450,7 +8407,7 @@
       <c r="C348" s="8"/>
       <c r="D348" s="8"/>
       <c r="E348" s="8"/>
-      <c r="F348" s="11"/>
+      <c r="F348" s="15"/>
       <c r="G348" s="12"/>
       <c r="H348" s="12"/>
       <c r="I348" s="12"/>
@@ -8469,7 +8426,7 @@
       <c r="C349" s="8"/>
       <c r="D349" s="8"/>
       <c r="E349" s="8"/>
-      <c r="F349" s="15"/>
+      <c r="F349" s="11"/>
       <c r="G349" s="12"/>
       <c r="H349" s="12"/>
       <c r="I349" s="12"/>
@@ -8488,7 +8445,7 @@
       <c r="C350" s="8"/>
       <c r="D350" s="8"/>
       <c r="E350" s="8"/>
-      <c r="F350" s="11"/>
+      <c r="F350" s="15"/>
       <c r="G350" s="12"/>
       <c r="H350" s="12"/>
       <c r="I350" s="12"/>
@@ -8526,7 +8483,7 @@
       <c r="C352" s="8"/>
       <c r="D352" s="8"/>
       <c r="E352" s="8"/>
-      <c r="F352" s="15"/>
+      <c r="F352" s="11"/>
       <c r="G352" s="12"/>
       <c r="H352" s="12"/>
       <c r="I352" s="12"/>
@@ -8583,7 +8540,7 @@
       <c r="C355" s="8"/>
       <c r="D355" s="8"/>
       <c r="E355" s="8"/>
-      <c r="F355" s="11"/>
+      <c r="F355" s="15"/>
       <c r="G355" s="12"/>
       <c r="H355" s="12"/>
       <c r="I355" s="12"/>
@@ -8602,7 +8559,7 @@
       <c r="C356" s="8"/>
       <c r="D356" s="8"/>
       <c r="E356" s="8"/>
-      <c r="F356" s="15"/>
+      <c r="F356" s="11"/>
       <c r="G356" s="12"/>
       <c r="H356" s="12"/>
       <c r="I356" s="12"/>
@@ -8697,7 +8654,7 @@
       <c r="C361" s="8"/>
       <c r="D361" s="8"/>
       <c r="E361" s="8"/>
-      <c r="F361" s="11"/>
+      <c r="F361" s="15"/>
       <c r="G361" s="12"/>
       <c r="H361" s="12"/>
       <c r="I361" s="12"/>
@@ -8716,7 +8673,7 @@
       <c r="C362" s="8"/>
       <c r="D362" s="8"/>
       <c r="E362" s="8"/>
-      <c r="F362" s="15"/>
+      <c r="F362" s="11"/>
       <c r="G362" s="12"/>
       <c r="H362" s="12"/>
       <c r="I362" s="12"/>
@@ -8735,7 +8692,7 @@
       <c r="C363" s="8"/>
       <c r="D363" s="8"/>
       <c r="E363" s="8"/>
-      <c r="F363" s="11"/>
+      <c r="F363" s="15"/>
       <c r="G363" s="12"/>
       <c r="H363" s="12"/>
       <c r="I363" s="12"/>
@@ -8754,7 +8711,7 @@
       <c r="C364" s="8"/>
       <c r="D364" s="8"/>
       <c r="E364" s="8"/>
-      <c r="F364" s="15"/>
+      <c r="F364" s="11"/>
       <c r="G364" s="12"/>
       <c r="H364" s="12"/>
       <c r="I364" s="12"/>
@@ -8830,7 +8787,7 @@
       <c r="C368" s="8"/>
       <c r="D368" s="8"/>
       <c r="E368" s="8"/>
-      <c r="F368" s="11"/>
+      <c r="F368" s="15"/>
       <c r="G368" s="12"/>
       <c r="H368" s="12"/>
       <c r="I368" s="12"/>
@@ -8925,7 +8882,7 @@
       <c r="C373" s="8"/>
       <c r="D373" s="8"/>
       <c r="E373" s="8"/>
-      <c r="F373" s="15"/>
+      <c r="F373" s="11"/>
       <c r="G373" s="12"/>
       <c r="H373" s="12"/>
       <c r="I373" s="12"/>
@@ -8944,7 +8901,7 @@
       <c r="C374" s="8"/>
       <c r="D374" s="8"/>
       <c r="E374" s="8"/>
-      <c r="F374" s="11"/>
+      <c r="F374" s="15"/>
       <c r="G374" s="12"/>
       <c r="H374" s="12"/>
       <c r="I374" s="12"/>
@@ -8963,7 +8920,7 @@
       <c r="C375" s="8"/>
       <c r="D375" s="8"/>
       <c r="E375" s="8"/>
-      <c r="F375" s="15"/>
+      <c r="F375" s="11"/>
       <c r="G375" s="12"/>
       <c r="H375" s="12"/>
       <c r="I375" s="12"/>
@@ -9001,7 +8958,7 @@
       <c r="C377" s="8"/>
       <c r="D377" s="8"/>
       <c r="E377" s="8"/>
-      <c r="F377" s="11"/>
+      <c r="F377" s="15"/>
       <c r="G377" s="12"/>
       <c r="H377" s="12"/>
       <c r="I377" s="12"/>
@@ -9096,7 +9053,7 @@
       <c r="C382" s="8"/>
       <c r="D382" s="8"/>
       <c r="E382" s="8"/>
-      <c r="F382" s="15"/>
+      <c r="F382" s="11"/>
       <c r="G382" s="12"/>
       <c r="H382" s="12"/>
       <c r="I382" s="12"/>
@@ -9134,7 +9091,7 @@
       <c r="C384" s="8"/>
       <c r="D384" s="8"/>
       <c r="E384" s="8"/>
-      <c r="F384" s="11"/>
+      <c r="F384" s="15"/>
       <c r="G384" s="12"/>
       <c r="H384" s="12"/>
       <c r="I384" s="12"/>
@@ -9153,7 +9110,7 @@
       <c r="C385" s="8"/>
       <c r="D385" s="8"/>
       <c r="E385" s="8"/>
-      <c r="F385" s="15"/>
+      <c r="F385" s="11"/>
       <c r="G385" s="12"/>
       <c r="H385" s="12"/>
       <c r="I385" s="12"/>
@@ -9191,7 +9148,7 @@
       <c r="C387" s="8"/>
       <c r="D387" s="8"/>
       <c r="E387" s="8"/>
-      <c r="F387" s="11"/>
+      <c r="F387" s="15"/>
       <c r="G387" s="12"/>
       <c r="H387" s="12"/>
       <c r="I387" s="12"/>
@@ -9210,7 +9167,7 @@
       <c r="C388" s="8"/>
       <c r="D388" s="8"/>
       <c r="E388" s="8"/>
-      <c r="F388" s="15"/>
+      <c r="F388" s="11"/>
       <c r="G388" s="12"/>
       <c r="H388" s="12"/>
       <c r="I388" s="12"/>
@@ -9229,7 +9186,7 @@
       <c r="C389" s="8"/>
       <c r="D389" s="8"/>
       <c r="E389" s="8"/>
-      <c r="F389" s="11"/>
+      <c r="F389" s="15"/>
       <c r="G389" s="12"/>
       <c r="H389" s="12"/>
       <c r="I389" s="12"/>
@@ -9248,7 +9205,7 @@
       <c r="C390" s="8"/>
       <c r="D390" s="8"/>
       <c r="E390" s="8"/>
-      <c r="F390" s="15"/>
+      <c r="F390" s="11"/>
       <c r="G390" s="12"/>
       <c r="H390" s="12"/>
       <c r="I390" s="12"/>
@@ -9269,7 +9226,7 @@
       <c r="E391" s="8"/>
       <c r="F391" s="11"/>
       <c r="G391" s="12"/>
-      <c r="H391" s="12"/>
+      <c r="H391" s="8"/>
       <c r="I391" s="12"/>
       <c r="J391" s="13"/>
       <c r="K391" s="13"/>
@@ -9402,7 +9359,7 @@
       <c r="E398" s="8"/>
       <c r="F398" s="11"/>
       <c r="G398" s="12"/>
-      <c r="H398" s="8"/>
+      <c r="H398" s="12"/>
       <c r="I398" s="12"/>
       <c r="J398" s="13"/>
       <c r="K398" s="13"/>
@@ -9421,7 +9378,7 @@
       <c r="E399" s="8"/>
       <c r="F399" s="11"/>
       <c r="G399" s="12"/>
-      <c r="H399" s="12"/>
+      <c r="H399" s="8"/>
       <c r="I399" s="12"/>
       <c r="J399" s="13"/>
       <c r="K399" s="13"/>
@@ -9457,9 +9414,9 @@
       <c r="C401" s="8"/>
       <c r="D401" s="8"/>
       <c r="E401" s="8"/>
-      <c r="F401" s="11"/>
+      <c r="F401" s="15"/>
       <c r="G401" s="12"/>
-      <c r="H401" s="8"/>
+      <c r="H401" s="12"/>
       <c r="I401" s="12"/>
       <c r="J401" s="13"/>
       <c r="K401" s="13"/>
@@ -9471,18 +9428,18 @@
       <c r="Q401" s="14"/>
     </row>
     <row r="402" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A402" s="8"/>
-      <c r="B402" s="8"/>
-      <c r="C402" s="8"/>
-      <c r="D402" s="8"/>
-      <c r="E402" s="8"/>
-      <c r="F402" s="15"/>
-      <c r="G402" s="12"/>
-      <c r="H402" s="12"/>
-      <c r="I402" s="12"/>
-      <c r="J402" s="13"/>
-      <c r="K402" s="13"/>
-      <c r="L402" s="8"/>
+      <c r="A402" s="3"/>
+      <c r="B402" s="4"/>
+      <c r="C402" s="5"/>
+      <c r="D402" s="5"/>
+      <c r="E402" s="4"/>
+      <c r="F402" s="6"/>
+      <c r="G402" s="7"/>
+      <c r="H402" s="7"/>
+      <c r="I402" s="4"/>
+      <c r="J402" s="8"/>
+      <c r="K402" s="8"/>
+      <c r="L402" s="4"/>
       <c r="M402" s="9"/>
       <c r="N402" s="14"/>
       <c r="O402" s="14"/>
@@ -9492,8 +9449,8 @@
     <row r="403" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A403" s="3"/>
       <c r="B403" s="4"/>
-      <c r="C403" s="5"/>
-      <c r="D403" s="5"/>
+      <c r="C403" s="10"/>
+      <c r="D403" s="10"/>
       <c r="E403" s="4"/>
       <c r="F403" s="6"/>
       <c r="G403" s="7"/>
@@ -9511,8 +9468,8 @@
     <row r="404" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A404" s="3"/>
       <c r="B404" s="4"/>
-      <c r="C404" s="10"/>
-      <c r="D404" s="10"/>
+      <c r="C404" s="5"/>
+      <c r="D404" s="5"/>
       <c r="E404" s="4"/>
       <c r="F404" s="6"/>
       <c r="G404" s="7"/>
@@ -9530,8 +9487,8 @@
     <row r="405" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A405" s="3"/>
       <c r="B405" s="4"/>
-      <c r="C405" s="5"/>
-      <c r="D405" s="5"/>
+      <c r="C405" s="10"/>
+      <c r="D405" s="10"/>
       <c r="E405" s="4"/>
       <c r="F405" s="6"/>
       <c r="G405" s="7"/>
@@ -9549,8 +9506,8 @@
     <row r="406" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A406" s="3"/>
       <c r="B406" s="4"/>
-      <c r="C406" s="10"/>
-      <c r="D406" s="10"/>
+      <c r="C406" s="5"/>
+      <c r="D406" s="5"/>
       <c r="E406" s="4"/>
       <c r="F406" s="6"/>
       <c r="G406" s="7"/>
@@ -9587,8 +9544,8 @@
     <row r="408" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A408" s="3"/>
       <c r="B408" s="4"/>
-      <c r="C408" s="5"/>
-      <c r="D408" s="5"/>
+      <c r="C408" s="10"/>
+      <c r="D408" s="10"/>
       <c r="E408" s="4"/>
       <c r="F408" s="6"/>
       <c r="G408" s="7"/>
@@ -9606,8 +9563,8 @@
     <row r="409" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A409" s="3"/>
       <c r="B409" s="4"/>
-      <c r="C409" s="10"/>
-      <c r="D409" s="10"/>
+      <c r="C409" s="5"/>
+      <c r="D409" s="5"/>
       <c r="E409" s="4"/>
       <c r="F409" s="6"/>
       <c r="G409" s="7"/>
@@ -9622,29 +9579,14 @@
       <c r="P409" s="14"/>
       <c r="Q409" s="14"/>
     </row>
-    <row r="410" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A410" s="3"/>
-      <c r="B410" s="4"/>
-      <c r="C410" s="5"/>
-      <c r="D410" s="5"/>
-      <c r="E410" s="4"/>
-      <c r="F410" s="6"/>
-      <c r="G410" s="7"/>
-      <c r="H410" s="7"/>
-      <c r="I410" s="4"/>
-      <c r="J410" s="8"/>
-      <c r="K410" s="8"/>
-      <c r="L410" s="4"/>
-      <c r="M410" s="9"/>
-      <c r="N410" s="14"/>
-      <c r="O410" s="14"/>
-      <c r="P410" s="14"/>
-      <c r="Q410" s="14"/>
+    <row r="410" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J410" s="14"/>
+      <c r="K410" s="14"/>
+      <c r="L410" s="17"/>
     </row>
     <row r="411" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="J411" s="14"/>
       <c r="K411" s="14"/>
-      <c r="L411" s="17"/>
     </row>
     <row r="412" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="J412" s="14"/>
@@ -10982,18 +10924,14 @@
       <c r="J745" s="14"/>
       <c r="K745" s="14"/>
     </row>
-    <row r="746" spans="10:11" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="J746" s="14"/>
-      <c r="K746" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M410" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M410">
-      <sortCondition ref="E1:E410"/>
+  <autoFilter ref="A1:M409" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M409">
+      <sortCondition ref="E1:E409"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M746">
-    <sortCondition ref="B1:B746"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M745">
+    <sortCondition ref="B1:B745"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>